<commit_message>
HxBank api debugging test
</commit_message>
<xml_diff>
--- a/doc/Api_array.xlsx
+++ b/doc/Api_array.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="15" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="6.1" sheetId="39" r:id="rId1"/>
@@ -2636,13 +2636,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2654,14 +2648,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -2670,6 +2664,15 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2689,9 +2692,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3026,22 +3026,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>400</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -3061,13 +3061,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -3116,7 +3116,7 @@
       <c r="D8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="36" t="s">
         <v>397</v>
       </c>
     </row>
@@ -3250,22 +3250,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -3285,13 +3285,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -3454,22 +3454,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -3489,13 +3489,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -4160,22 +4160,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -4195,13 +4195,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -4458,22 +4458,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -4493,13 +4493,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -4647,22 +4647,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -4682,13 +4682,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -5012,22 +5012,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -5047,13 +5047,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -5214,22 +5214,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -5249,13 +5249,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -5480,22 +5480,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -5515,13 +5515,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -5667,22 +5667,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>248</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -5702,13 +5702,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="41"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -5883,7 +5883,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5914,22 +5914,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -5949,64 +5949,72 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>50</v>
+      <c r="A7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="A8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>95</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>96</v>
+        <v>180</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>0</v>
@@ -6015,13 +6023,13 @@
     </row>
     <row r="10" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>0</v>
@@ -6030,57 +6038,59 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>182</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>183</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
@@ -6089,47 +6099,30 @@
         <v>15</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6141,7 +6134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6168,22 +6161,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>402</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -6203,13 +6196,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -6455,9 +6448,11 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -6486,22 +6481,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>257</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -6521,81 +6516,89 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>50</v>
+      <c r="A7" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>73</v>
+      <c r="A8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>253</v>
-      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>0</v>
@@ -6604,13 +6607,13 @@
     </row>
     <row r="11" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>0</v>
@@ -6619,40 +6622,42 @@
     </row>
     <row r="12" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>53</v>
+        <v>254</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>181</v>
+        <v>255</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>254</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -6661,47 +6666,30 @@
         <v>15</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A5:E5"/>
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -6745,22 +6733,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -6780,13 +6768,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -6881,22 +6869,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="126.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -6916,13 +6904,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -7214,22 +7202,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>284</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -7249,13 +7237,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -7401,22 +7389,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>287</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -7436,13 +7424,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -7608,22 +7596,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -7643,13 +7631,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -7744,22 +7732,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -7779,13 +7767,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -7946,22 +7934,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>302</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -7981,13 +7969,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -8229,22 +8217,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>306</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -8264,13 +8252,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -8415,9 +8403,9 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8446,22 +8434,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>319</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -8481,13 +8469,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -8590,21 +8578,29 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>96</v>
+        <v>202</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>0</v>
@@ -8613,13 +8609,13 @@
     </row>
     <row r="14" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>0</v>
@@ -8628,91 +8624,93 @@
     </row>
     <row r="15" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>158</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>203</v>
+        <v>311</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>3</v>
+        <v>312</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>311</v>
+        <v>39</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>312</v>
+        <v>183</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>313</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>183</v>
+        <v>230</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>31</v>
+      <c r="A18" s="35" t="s">
+        <v>314</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>315</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>230</v>
+        <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
-        <v>314</v>
+      <c r="A19" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>315</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>316</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -8721,40 +8719,23 @@
         <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -8800,22 +8781,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -8835,13 +8816,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -8990,22 +8971,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>324</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -9025,13 +9006,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -9177,22 +9158,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>328</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -9212,13 +9193,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -9458,22 +9439,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>332</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -9493,13 +9474,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -9647,22 +9628,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -9682,13 +9663,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -9909,22 +9890,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>338</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -9944,13 +9925,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -10190,22 +10171,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>340</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -10225,13 +10206,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -10471,22 +10452,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>358</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="43" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -10506,13 +10487,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -10891,22 +10872,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="49" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>369</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -10926,13 +10907,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -11110,22 +11091,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>373</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>374</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -11145,13 +11126,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -11344,22 +11325,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>380</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>381</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -11379,13 +11360,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -11548,22 +11529,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -11583,13 +11564,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -11772,22 +11753,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
@@ -11807,13 +11788,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -12057,22 +12038,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -12092,13 +12073,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -12246,22 +12227,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -12281,13 +12262,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -12530,22 +12511,22 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="51"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -12565,13 +12546,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -12734,20 +12715,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="44"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -12767,13 +12748,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">

</xml_diff>